<commit_message>
adding our details- Nitay man
</commit_message>
<xml_diff>
--- a/Administration/submission groups.xlsx
+++ b/Administration/submission groups.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EA4350-E5C0-4AB8-82F0-35D03303B0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" codeName="חוברת_עבודה_זו"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8574BB2-9483-4F62-AC74-E58B7C40D878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="11" sheetId="1" r:id="rId1"/>
@@ -16,17 +16,28 @@
     <sheet name="16" sheetId="6" r:id="rId6"/>
     <sheet name="17" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>esti leykind</t>
   </si>
@@ -38,6 +49,18 @@
   </si>
   <si>
     <t>yonatan reznik</t>
+  </si>
+  <si>
+    <t>Daniel Magnezi</t>
+  </si>
+  <si>
+    <t>Dniel Mani</t>
+  </si>
+  <si>
+    <t>Ofri Serussi</t>
+  </si>
+  <si>
+    <t>Nitay Man</t>
   </si>
 </sst>
 </file>
@@ -48,7 +71,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -355,13 +378,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="גיליון1"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -369,62 +393,86 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D780CD77-293F-46EC-982D-8D3272935F27}">
+  <sheetPr codeName="גיליון2"/>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB0A5F5-9C5D-4818-B4E3-CF7DD873C58B}">
+  <sheetPr codeName="גיליון3"/>
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB0A5F5-9C5D-4818-B4E3-CF7DD873C58B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC2C2EC-4C05-4B7A-ACF5-F6DC153EB164}">
+  <sheetPr codeName="גיליון4"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -432,13 +480,14 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2E1B68-FE15-4E75-B7A6-63B0E75BA1CE}">
+  <sheetPr codeName="גיליון5"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -446,13 +495,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43CD0B6F-0567-4281-BE54-0E2D34CD542D}">
+  <sheetPr codeName="גיליון6"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -460,13 +510,14 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA65734F-1BB6-4740-AED5-75ABD12BEB34}">
+  <sheetPr codeName="גיליון7"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding a new file by nitzanbutbul
</commit_message>
<xml_diff>
--- a/Administration/submission groups.xlsx
+++ b/Administration/submission groups.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
-  <workbookPr filterPrivacy="1" codeName="חוברת_עבודה_זו"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8574BB2-9483-4F62-AC74-E58B7C40D878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" codeName="חוברת_עבודה_זו" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
-    <sheet name="11" sheetId="1" r:id="rId1"/>
-    <sheet name="12" sheetId="2" r:id="rId2"/>
-    <sheet name="13" sheetId="3" r:id="rId3"/>
-    <sheet name="14" sheetId="4" r:id="rId4"/>
-    <sheet name="15" sheetId="5" r:id="rId5"/>
-    <sheet name="16" sheetId="6" r:id="rId6"/>
-    <sheet name="17" sheetId="7" r:id="rId7"/>
+    <sheet name="9" sheetId="8" r:id="rId1"/>
+    <sheet name="11" sheetId="1" r:id="rId2"/>
+    <sheet name="12" sheetId="2" r:id="rId3"/>
+    <sheet name="13" sheetId="3" r:id="rId4"/>
+    <sheet name="14" sheetId="4" r:id="rId5"/>
+    <sheet name="15" sheetId="5" r:id="rId6"/>
+    <sheet name="16" sheetId="6" r:id="rId7"/>
+    <sheet name="17" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>esti leykind</t>
   </si>
@@ -62,11 +62,23 @@
   <si>
     <t>Nitay Man</t>
   </si>
+  <si>
+    <t>Nitzan Butbul</t>
+  </si>
+  <si>
+    <t>Hadar Dahan</t>
+  </si>
+  <si>
+    <t>Shelly Safrai</t>
+  </si>
+  <si>
+    <t>Yuval Melamed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -377,7 +389,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="גיליון1"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -385,39 +432,39 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D780CD77-293F-46EC-982D-8D3272935F27}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="גיליון2"/>
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -427,33 +474,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB0A5F5-9C5D-4818-B4E3-CF7DD873C58B}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="גיליון3"/>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -463,8 +510,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC2C2EC-4C05-4B7A-ACF5-F6DC153EB164}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="גיליון4"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -472,14 +519,14 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2E1B68-FE15-4E75-B7A6-63B0E75BA1CE}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="גיליון5"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -487,14 +534,14 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43CD0B6F-0567-4281-BE54-0E2D34CD542D}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="גיליון6"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -502,14 +549,14 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA65734F-1BB6-4740-AED5-75ABD12BEB34}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="גיליון7"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -517,7 +564,7 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added our details to submission groups file
</commit_message>
<xml_diff>
--- a/Administration/submission groups.xlsx
+++ b/Administration/submission groups.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="חוברת_עבודה_זו"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8574BB2-9483-4F62-AC74-E58B7C40D878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F359120-CA87-4099-A9F7-5752688B53C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-8805" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="11" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>esti leykind</t>
   </si>
@@ -61,13 +61,57 @@
   </si>
   <si>
     <t>Nitay Man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Names </t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group number </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>group number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Gal Etach</t>
+  </si>
+  <si>
+    <t>Shani Gueta</t>
+  </si>
+  <si>
+    <t>Ron Bitan</t>
+  </si>
+  <si>
+    <t>Ofri Ben David</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,13 +119,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -96,8 +169,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,7 +469,7 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -400,24 +484,24 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -430,36 +514,95 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB0A5F5-9C5D-4818-B4E3-CF7DD873C58B}">
   <sheetPr codeName="גיליון3"/>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.58203125" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="5"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2">
+        <v>315864694</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2">
+        <v>208499186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -472,7 +615,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -487,7 +630,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -502,7 +645,7 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -517,7 +660,7 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added group 13 to sheet 11
</commit_message>
<xml_diff>
--- a/Administration/submission groups.xlsx
+++ b/Administration/submission groups.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" codeName="חוברת_עבודה_זו"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292B6998-01EC-470A-BE53-D67734098F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14B8295-F540-4EFE-B157-75EC95BCA0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="830" windowWidth="14400" windowHeight="7370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="11" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>esti leykind</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>Paz Elraz</t>
+  </si>
+  <si>
+    <t>Bar Eckstien</t>
+  </si>
+  <si>
+    <t>Itai Orr</t>
+  </si>
+  <si>
+    <t>Ofri Efrati</t>
+  </si>
+  <si>
+    <t>Liav Teplizkiy</t>
   </si>
 </sst>
 </file>
@@ -391,14 +403,35 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="גיליון1"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -408,7 +441,7 @@
   <sheetPr codeName="גיליון2"/>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updating names on excel file
</commit_message>
<xml_diff>
--- a/Administration/submission groups.xlsx
+++ b/Administration/submission groups.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" codeName="חוברת_עבודה_זו"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DE2FA3-DA8E-462C-9E68-C0669FE6FBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283705D3-3272-46E0-B866-76FC5A5DAC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="11" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>esti leykind</t>
   </si>
@@ -85,6 +84,15 @@
   </si>
   <si>
     <t>Reut Goldman</t>
+  </si>
+  <si>
+    <t>Alon Nadel</t>
+  </si>
+  <si>
+    <t>Bar Naor</t>
+  </si>
+  <si>
+    <t>Gil Tamir</t>
   </si>
 </sst>
 </file>
@@ -95,7 +103,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -409,7 +417,7 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -424,7 +432,7 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -472,7 +480,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -502,14 +510,30 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC2C2EC-4C05-4B7A-ACF5-F6DC153EB164}">
   <sheetPr codeName="גיליון4"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -519,11 +543,11 @@
   <sheetPr codeName="גיליון5"/>
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -559,7 +583,7 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -574,7 +598,7 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added group 18 submission
</commit_message>
<xml_diff>
--- a/Administration/submission groups.xlsx
+++ b/Administration/submission groups.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="חוברת_עבודה_זו"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283705D3-3272-46E0-B866-76FC5A5DAC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9937E1-EB9D-41A6-A5B6-A1B79BC48905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="11" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>esti leykind</t>
   </si>
@@ -93,6 +93,15 @@
   </si>
   <si>
     <t>Gil Tamir</t>
+  </si>
+  <si>
+    <t>Lior Malik</t>
+  </si>
+  <si>
+    <t>Astar Avraham</t>
+  </si>
+  <si>
+    <t>Noa Malka</t>
   </si>
 </sst>
 </file>
@@ -103,7 +112,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -417,7 +426,7 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -432,7 +441,7 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -480,7 +489,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -512,11 +521,11 @@
   <sheetPr codeName="גיליון4"/>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -541,13 +550,13 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E2E1B68-FE15-4E75-B7A6-63B0E75BA1CE}">
   <sheetPr codeName="גיליון5"/>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -567,6 +576,21 @@
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -583,7 +607,7 @@
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -598,7 +622,7 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding our names by G
</commit_message>
<xml_diff>
--- a/Administration/submission groups.xlsx
+++ b/Administration/submission groups.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" codeName="חוברת_עבודה_זו"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283705D3-3272-46E0-B866-76FC5A5DAC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDAAB6B-5F4F-4FB5-8887-A0F1C6AC2588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5220" yWindow="528" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="11" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>esti leykind</t>
   </si>
@@ -93,6 +93,18 @@
   </si>
   <si>
     <t>Gil Tamir</t>
+  </si>
+  <si>
+    <t>Gabreal haj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amitay Lavi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michal Yonasi </t>
+  </si>
+  <si>
+    <t>Yaniv Avraham</t>
   </si>
 </sst>
 </file>
@@ -474,32 +486,44 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB0A5F5-9C5D-4818-B4E3-CF7DD873C58B}">
   <sheetPr codeName="גיליון3"/>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -512,7 +536,7 @@
   <sheetPr codeName="גיליון4"/>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>